<commit_message>
Issue #1 / SQID has a Database now.  Grids load GOBs now
</commit_message>
<xml_diff>
--- a/data/StuffQuest Game Data.xlsx
+++ b/data/StuffQuest Game Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\My Stuff\Projects\StuffQuest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A01CE-DB06-472B-9E0E-D88942BD39CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5CB7EB-C0DE-42D1-9618-B025566D85FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{15129302-3F60-48B0-BE7A-F5DC3552919F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26970" windowHeight="16440" activeTab="2" xr2:uid="{15129302-3F60-48B0-BE7A-F5DC3552919F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
     <sheet name="Grid" sheetId="1" r:id="rId2"/>
-    <sheet name="Portal" sheetId="2" r:id="rId3"/>
+    <sheet name="Conduit" sheetId="2" r:id="rId3"/>
+    <sheet name="Portal" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>a48a9f74-2303-4f29-b7ab-01e796ae7cf2</t>
   </si>
@@ -250,7 +251,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -378,17 +379,17 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -404,24 +405,32 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="20">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Bahnschrift Light Condensed"/>
+        <name val="Bahnschrift SemiCondensed"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -440,6 +449,46 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -465,15 +514,33 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -529,7 +596,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -549,7 +615,89 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift SemiCondensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light Condensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -598,8 +746,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9DC8550-E367-42E5-9AB3-6B54F4293B9F}" name="Table1" displayName="Table1" ref="A1:B32" totalsRowShown="0">
   <autoFilter ref="A1:B32" xr:uid="{795A3259-AF9D-4325-8403-B5A6F3C7AC4B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A24F164B-EA81-4933-92E4-3F9300230EC1}" name="uuid" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{2B9917AD-A0F9-474F-ACA8-62DEAA9DE5BE}" name="description" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{A24F164B-EA81-4933-92E4-3F9300230EC1}" name="uuid" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{2B9917AD-A0F9-474F-ACA8-62DEAA9DE5BE}" name="description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -615,18 +763,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{208703EB-60F5-4FB5-BC20-9B5314B41FBA}" name="uuid" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{806FC132-CBBD-4ADC-91AB-5CEEC5010908}" name="in x" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{6E1516D8-6922-4309-B05D-D021FBFD09E6}" name="in y" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{90A83388-B70F-47E8-8940-4DFD0CA546E9}" name="in uuid" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{8FE17454-97AD-446B-9E49-8E060E935556}" name="in grid" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{208703EB-60F5-4FB5-BC20-9B5314B41FBA}" name="uuid" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{806FC132-CBBD-4ADC-91AB-5CEEC5010908}" name="in x" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{6E1516D8-6922-4309-B05D-D021FBFD09E6}" name="in y" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{90A83388-B70F-47E8-8940-4DFD0CA546E9}" name="in uuid" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{8FE17454-97AD-446B-9E49-8E060E935556}" name="in grid" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AFA8722E-C61A-4B36-A46D-89A62357A3FD}" name="out x" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{0A103C36-ADE6-4673-8477-02070E1A43AB}" name="out y" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{6A3AF3E9-C6BA-4336-AAB5-D3654B9E9CA2}" name="out uuid" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{3C9F1CF5-E21A-4D36-A7A5-3293315CB047}" name="out grid" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{AFA8722E-C61A-4B36-A46D-89A62357A3FD}" name="out x" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{0A103C36-ADE6-4673-8477-02070E1A43AB}" name="out y" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{6A3AF3E9-C6BA-4336-AAB5-D3654B9E9CA2}" name="out uuid" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{3C9F1CF5-E21A-4D36-A7A5-3293315CB047}" name="out grid" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{584223A4-B62A-45CB-A243-4933A7239311}" name="PortalTable4" displayName="PortalTable4" ref="A1:I24" totalsRowShown="0">
+  <autoFilter ref="A1:I24" xr:uid="{795A3259-AF9D-4325-8403-B5A6F3C7AC4B}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Beregost"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D6D10D17-0833-474F-82EC-A39570F56047}" name="uuid" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{12C9C6C9-7FE5-41A0-8057-8AE4BA1B41B3}" name="in x" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{C326BEDF-56B8-4C1D-8F50-185A150CA919}" name="in y" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1F08E108-1949-411B-9157-438B1328EF8F}" name="in uuid" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4CE0C796-1619-4D79-8BA1-92E17CCA516D}" name="in grid" dataDxfId="4">
+      <calculatedColumnFormula>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{5516FF0E-5465-4AD6-B4DB-B66B3D092006}" name="out x" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{F1762B65-FA40-4D81-93E6-8A783DBC8BEF}" name="out y" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{869CE228-0F94-4419-BDBF-90E310FF64E9}" name="out uuid" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{32776A2D-96A8-48A1-A5FE-E4B3477ACA8A}" name="out grid" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1190,6 +1366,536 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>Beregost</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="10" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>Feldpost's Inn</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>Feldpost's Inn</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>Beregost</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>Beregost</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="16" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>Temple</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>Beregost</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>Beregost</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="14" t="str">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>Coast Way</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="14" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="16" t="e">
+        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4E0116-3DD7-4FE9-97FB-E789130D207D}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1248,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="9" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>Beregost</v>
       </c>
       <c r="F2" s="11">
@@ -1261,7 +1967,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="10" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>Feldpost's Inn</v>
       </c>
     </row>
@@ -1279,7 +1985,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="9" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>Feldpost's Inn</v>
       </c>
       <c r="F3" s="11">
@@ -1292,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="10" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>Beregost</v>
       </c>
     </row>
@@ -1306,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="14" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>Beregost</v>
       </c>
       <c r="F4" s="15"/>
@@ -1315,7 +2021,7 @@
         <v>14</v>
       </c>
       <c r="I4" s="16" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>Temple</v>
       </c>
     </row>
@@ -1329,14 +2035,14 @@
         <v>0</v>
       </c>
       <c r="E5" s="14" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>Beregost</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="5"/>
       <c r="I5" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1350,14 +2056,14 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>Beregost</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="5"/>
       <c r="I6" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1369,14 +2075,14 @@
       <c r="C7" s="13"/>
       <c r="D7" s="5"/>
       <c r="E7" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="5"/>
       <c r="I7" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1390,14 +2096,14 @@
         <v>16</v>
       </c>
       <c r="E8" s="14" t="str">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>Coast Way</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="5"/>
       <c r="I8" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1409,14 +2115,14 @@
       <c r="C9" s="13"/>
       <c r="D9" s="5"/>
       <c r="E9" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="5"/>
       <c r="I9" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1428,14 +2134,14 @@
       <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="E10" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="5"/>
       <c r="I10" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1447,14 +2153,14 @@
       <c r="C11" s="13"/>
       <c r="D11" s="5"/>
       <c r="E11" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="5"/>
       <c r="I11" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1466,14 +2172,14 @@
       <c r="C12" s="13"/>
       <c r="D12" s="5"/>
       <c r="E12" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="5"/>
       <c r="I12" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1485,14 +2191,14 @@
       <c r="C13" s="13"/>
       <c r="D13" s="5"/>
       <c r="E13" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="5"/>
       <c r="I13" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1504,14 +2210,14 @@
       <c r="C14" s="13"/>
       <c r="D14" s="5"/>
       <c r="E14" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="5"/>
       <c r="I14" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1523,14 +2229,14 @@
       <c r="C15" s="13"/>
       <c r="D15" s="5"/>
       <c r="E15" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="5"/>
       <c r="I15" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1542,14 +2248,14 @@
       <c r="C16" s="13"/>
       <c r="D16" s="5"/>
       <c r="E16" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="5"/>
       <c r="I16" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1561,14 +2267,14 @@
       <c r="C17" s="13"/>
       <c r="D17" s="5"/>
       <c r="E17" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="5"/>
       <c r="I17" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1580,14 +2286,14 @@
       <c r="C18" s="13"/>
       <c r="D18" s="5"/>
       <c r="E18" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="5"/>
       <c r="I18" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1599,14 +2305,14 @@
       <c r="C19" s="13"/>
       <c r="D19" s="5"/>
       <c r="E19" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="5"/>
       <c r="I19" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1618,14 +2324,14 @@
       <c r="C20" s="13"/>
       <c r="D20" s="5"/>
       <c r="E20" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="5"/>
       <c r="I20" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1637,14 +2343,14 @@
       <c r="C21" s="13"/>
       <c r="D21" s="5"/>
       <c r="E21" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="5"/>
       <c r="I21" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1656,14 +2362,14 @@
       <c r="C22" s="13"/>
       <c r="D22" s="5"/>
       <c r="E22" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="5"/>
       <c r="I22" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1675,14 +2381,14 @@
       <c r="C23" s="13"/>
       <c r="D23" s="5"/>
       <c r="E23" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="5"/>
       <c r="I23" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -1694,19 +2400,18 @@
       <c r="C24" s="13"/>
       <c r="D24" s="5"/>
       <c r="E24" s="14" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[in uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="5"/>
       <c r="I24" s="16" t="e">
-        <f>VLOOKUP(PortalTable[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
+        <f>VLOOKUP(PortalTable4[[#This Row],[out uuid]],Table1[],2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>